<commit_message>
Updated data template and tasks form
</commit_message>
<xml_diff>
--- a/project_mgmt/case_cities_data.xlsx
+++ b/project_mgmt/case_cities_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmtg3\OneDrive\Cambridge\TIGTHAT\ITHIM-R\project_mgmt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="152" documentId="13_ncr:1_{58B9BE8B-73DC-4B84-B270-ADD34A1BB702}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{4512EEF0-1C7D-40C1-9BF5-210A5B2A4FDC}"/>
+  <xr:revisionPtr revIDLastSave="211" documentId="13_ncr:1_{58B9BE8B-73DC-4B84-B270-ADD34A1BB702}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{13226F7D-9110-4D89-A4D8-E344B46DA5C8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="211">
   <si>
     <t>Country</t>
   </si>
@@ -301,9 +301,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Ghana Population and Housing Census</t>
-  </si>
-  <si>
     <t>Background population data for the city</t>
   </si>
   <si>
@@ -427,9 +424,6 @@
     <t>2009-2010</t>
   </si>
   <si>
-    <t>Multiple files. Buenos Aires Metropolitan Area.</t>
-  </si>
-  <si>
     <t>National Department of Transportation</t>
   </si>
   <si>
@@ -508,33 +502,15 @@
     <t>Emailed by Ashish Verma from Bangalore</t>
   </si>
   <si>
-    <t>https://github.com/ITHIM/ITHIM-R/tree/master/inst/extdata/local/sao_paulo</t>
-  </si>
-  <si>
-    <t>https://github.com/ITHIM/ITHIM-R/tree/master/inst/extdata/local/accra</t>
-  </si>
-  <si>
-    <t>2005 &amp; 2015</t>
-  </si>
-  <si>
     <t>Our area is Valley of Mexico Metropolitan Area, formed by 61 cities: Acolman, Amecameca, Apaxco, Atenco, Atizapán de Zaragoza, Atlautla, Axapusco, Ayapango, Chalco, Chiautla, Chicoloapan, Chiconcuac, Chimalhuacán, Coacalco de Berriozábal, Cocotitlán, Coyotepec, Cuautitlán, Cuautitlán Izcalli, Ecatepec de Morelos, Ecatzingo, Huehuetoca, Hueypoxtla, Huixquilucan, Isidro Fabela, Ixtapaluca, Jaltenco, Jilotzingo, Juchitepec, La Paz, Melchor Ocampo, Mexico City, Naucalpan de Juárez, Nextlalpan, Nezahualcóyotl, Nicolás Romero, Nopaltepec, Otumba, Ozumba, Papalotla, San Martín de las Pirámides, Tecámac, Temamatla, Temascalapa, Tenango del Aire, Teoloyucan, Teotihuacán, Tepetlaoxtoc, Tepetlixpa, Tepotzotlán, Tequixquiac, Texcoco, Tezoyuca, Tizayuca, Tlalmanalco, Tlalnepantla de Baz, Tonanitla, Tultepec, Tultitlán, Valle de Chalco Solidaridad, Villa del Carbón, Zumpango.</t>
   </si>
   <si>
-    <t>Census Mexico</t>
-  </si>
-  <si>
-    <t>Census Chile</t>
-  </si>
-  <si>
     <t>Our area is Greater Accra Metropolitan Area, formed by 12 districts: Accra Metropolitan District, Tema Metropolis, Adenta, Ga East, Ga West, Ga South, Ga Central, La Nkwantang-Madina, Ledzokuku-Krowor, Ashaiman, Kpone-Katamanso, La Dade-Kotopon.</t>
   </si>
   <si>
     <t>Our area is Santiago Metropolitan Area, formed by 52 cities:  Alhué, Buin, Calera de Tango, Cerrillos, Cerro Navia, Colina, Conchalí, Curacaví, El Bosque, El Monte, Estación Central, Huechuraba, Independencia, Isla de Maipo, La Cisterna, La Florida, La Granja, La Pintana, La Reina, Lampa, Las Condes, Lo Barnechea, Lo Espejo, Lo Prado, Macul, Maipú, María Pinto, Melipilla, Ñuñoa, Padre Hurtado, Paine, Pedro Aguirre Cerda, Peñaflor, Peñalolén, Pirque, Providencia, Pudahuel, Puente Alto, Quilicura, Quinta Normal, Recoleta, Renca, San Bernardo, San Joaquín, San José de Maipo, San Miguel, San Pedro, San Ramón, Santiago, Talagante, Til Til, Vitacura</t>
   </si>
   <si>
-    <t>Census Argentina</t>
-  </si>
-  <si>
     <t>Belo Horizonte</t>
   </si>
   <si>
@@ -542,12 +518,6 @@
   </si>
   <si>
     <t xml:space="preserve"> ‎Port Louis</t>
-  </si>
-  <si>
-    <t>Our area is Buenos Aires Metropolitan Area, formed by 43 cities: Almirante Brown, Avellaneda, Berazategui, Berisso, Brandsen, Buenos Aires, Campana, Cañuelas, Ensenada, Escobar, Esteban Echeverría, Exaltación de la Cruz, Ezeiza, Florencio Varela, General Las Heras, General Rodríguez, General San Martín, Hurlingham, Ituzaingó, José C. Paz, La Matanza (parte este), La Matanza (parte oeste), La Plata, Lanús, Lomas de Zamora, Luján, Malvinas Argentinas, Marcos Paz, Merlo, Moreno, Morón, Pilar, Presidente Perón, Quilmes, San Fernando (parte continental), San Fernando (parte insular), San Isidro, San Miguel, San Vicente, Tigre, Tres de Febrero, Vicente López, Zárate.</t>
-  </si>
-  <si>
-    <t>Our area is Bogota D.C. only</t>
   </si>
   <si>
     <t>Sample size</t>
@@ -640,24 +610,12 @@
     </r>
   </si>
   <si>
-    <t>Two options available at least: WHO SAGE 2014 (wave 2), Physical Activity and Sports Survey 2013-2018 (https://www.inegi.org.mx/programas/mopradef/)</t>
-  </si>
-  <si>
-    <t>Census (2005) &amp; population projection (2015)</t>
-  </si>
-  <si>
     <t>2010 &amp; 2017</t>
   </si>
   <si>
     <t>Our area is Sao Paulo Metropolitan Area, formed by 34 cities: Baldim, Belo Horizonte, Betim, Brumadinho, Caeté, Capim Branco, Confins, Contagem, Esmeraldas, Florestal, Ibirité, Igarapé, Itaguara, Itatiaiuçu, Jaboticatubas, Nova União, Juatuba, Lagoa Santa, Mário Campos, Mateus Leme, Matozinhos, Nova Lima, Pedro Leopoldo, Raposos, Ribeirão das Neves, Rio Acima, Rio Manso, Sabará, Santa Luzia, São Joaquim de Bicas, São José da Lapa, Sarzedo, Taquaraçu de Minas, Vespasiano</t>
   </si>
   <si>
-    <t>https://github.com/ITHIM/ITHIM-R/tree/master/inst/extdata/local/belo_horizonte</t>
-  </si>
-  <si>
-    <t>Brazil Population and Housing Census (2010) &amp; population projection (2017) (both from the Brazilian Institute of Geography and Statistics)</t>
-  </si>
-  <si>
     <t>Development Agency of the Belo Horizonte Metropolitan Area</t>
   </si>
   <si>
@@ -698,6 +656,57 @@
   </si>
   <si>
     <t>V:\Studies\MOVED\HealthImpact\Data\TIGTHAT\Brazil\Road deaths 27 Brazilian capitals 2010-15.xlsx</t>
+  </si>
+  <si>
+    <t>Population projection</t>
+  </si>
+  <si>
+    <t>Our area is Bogota D.C. only. Last census done in 2005</t>
+  </si>
+  <si>
+    <t>Ghana Population and Housing Census (2010) &amp; population projection (2017)</t>
+  </si>
+  <si>
+    <t>Brazil Population and Housing Census (2010) &amp; population projection (2017)</t>
+  </si>
+  <si>
+    <t>Argentina Population and Housing Census (2010) &amp; population projection (2017)</t>
+  </si>
+  <si>
+    <t>Our area is Gran Buenos Aires, formed by 24 cities: Almirante Brown, Avellaneda, Berazategui, Esteban Echeverría, Ezeiza, Florencio Varela, General San Martín, Hurlingham, Ituzaingó, José C. Paz, La Matanza, Lanús, Lomas de Zamora, Malvinas Argentinas, Merlo, Moreno, Morón, Quilmes, San Fernando, San Isidro, San Miguel, Tigre, Tres de Febrero, Vicente López. Sex- and age-specific population projections for the Buenos Aires province.</t>
+  </si>
+  <si>
+    <t>Chile Population and Housing Census</t>
+  </si>
+  <si>
+    <t>Multiple files. Buenos Aires Metropolitan Area (larger than Gran Buenos Aires).</t>
+  </si>
+  <si>
+    <t>Mexico Population and Housing Census (2010) &amp; population projection (2017)</t>
+  </si>
+  <si>
+    <t>V:\Studies\MOVED\HealthImpact\Data\TIGTHAT\Accra\Accra data and microdata\Census</t>
+  </si>
+  <si>
+    <t>V:\Studies\MOVED\HealthImpact\Data\TIGTHAT\Brazil\Sao Paulo\Population</t>
+  </si>
+  <si>
+    <t>V:\Studies\MOVED\HealthImpact\Data\TIGTHAT\Brazil\Belo Horizonte\Population</t>
+  </si>
+  <si>
+    <t>V:\Studies\MOVED\HealthImpact\Data\TIGTHAT\Colombia\Bogota\Population</t>
+  </si>
+  <si>
+    <t>V:\Studies\MOVED\HealthImpact\Data\TIGTHAT\Mexico\Mexico City population</t>
+  </si>
+  <si>
+    <t>V:\Studies\MOVED\HealthImpact\Data\TIGTHAT\Argentina\Population</t>
+  </si>
+  <si>
+    <t>V:\Studies\MOVED\HealthImpact\Data\TIGTHAT\Chile\Population</t>
+  </si>
+  <si>
+    <t>Study on Global Aging and Adult Health (SAGE) - Wave 2</t>
   </si>
 </sst>
 </file>
@@ -1407,7 +1416,7 @@
   <dimension ref="A1:AL16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" sqref="A1:B1"/>
@@ -1422,11 +1431,11 @@
   <sheetData>
     <row r="1" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D1" s="34"/>
       <c r="E1" s="34"/>
@@ -1434,7 +1443,7 @@
       <c r="G1" s="34"/>
       <c r="H1" s="35"/>
       <c r="I1" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J1" s="33"/>
       <c r="K1" s="33"/>
@@ -1442,7 +1451,7 @@
       <c r="M1" s="33"/>
       <c r="N1" s="33"/>
       <c r="O1" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P1" s="34"/>
       <c r="Q1" s="34"/>
@@ -1464,7 +1473,7 @@
       <c r="AE1" s="33"/>
       <c r="AF1" s="36"/>
       <c r="AG1" s="34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AH1" s="34"/>
       <c r="AI1" s="34"/>
@@ -1525,7 +1534,7 @@
         <v>35</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="S2" s="5" t="s">
         <v>38</v>
@@ -1537,7 +1546,7 @@
         <v>37</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="W2" s="5" t="s">
         <v>40</v>
@@ -1552,7 +1561,7 @@
         <v>35</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="AB2" s="6" t="s">
         <v>38</v>
@@ -1564,7 +1573,7 @@
         <v>37</v>
       </c>
       <c r="AE2" s="6" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="AF2" s="6" t="s">
         <v>40</v>
@@ -1596,13 +1605,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="14">
-        <v>2010</v>
+        <v>196</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>178</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>159</v>
+        <v>203</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>78</v>
@@ -1611,7 +1620,7 @@
         <v>69</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="I3" s="16" t="s">
         <v>79</v>
@@ -1643,14 +1652,14 @@
         <v>70</v>
       </c>
       <c r="T3" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="U3" s="14" t="s">
         <v>69</v>
       </c>
       <c r="V3" s="14"/>
       <c r="W3" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="X3" s="16" t="s">
         <v>72</v>
@@ -1668,28 +1677,28 @@
         <v>76</v>
       </c>
       <c r="AC3" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AD3" s="16" t="s">
         <v>69</v>
       </c>
       <c r="AE3" s="16" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="AF3" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AG3" s="14" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="AH3" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AI3" s="14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AJ3" s="14" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="AK3" s="14" t="s">
         <v>69</v>
@@ -1704,13 +1713,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>158</v>
+        <v>204</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>78</v>
@@ -1719,7 +1728,7 @@
         <v>69</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I4" s="11" t="s">
         <v>79</v>
@@ -1735,75 +1744,75 @@
       </c>
       <c r="M4" s="11"/>
       <c r="N4" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P4" s="9">
         <v>2012</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R4" s="9"/>
       <c r="S4" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T4" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="U4" s="9" t="s">
         <v>69</v>
       </c>
       <c r="V4" s="9"/>
       <c r="W4" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="X4" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Y4" s="11">
         <v>2015</v>
       </c>
       <c r="Z4" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AA4" s="11">
         <v>3082</v>
       </c>
       <c r="AB4" s="11" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="AC4" s="11" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="AD4" s="11" t="s">
         <v>69</v>
       </c>
       <c r="AE4" s="11" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="AF4" s="11" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="AG4" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AH4" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI4" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="AI4" s="9" t="s">
+      <c r="AJ4" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="AJ4" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="AK4" s="9" t="s">
         <v>69</v>
       </c>
       <c r="AL4" s="21" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:38" s="2" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1811,16 +1820,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>78</v>
@@ -1829,7 +1838,7 @@
         <v>69</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="I5" s="16" t="s">
         <v>79</v>
@@ -1845,66 +1854,66 @@
       </c>
       <c r="M5" s="11"/>
       <c r="N5" s="11" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="P5" s="9">
         <v>2012</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="R5" s="9"/>
       <c r="S5" s="9" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="T5" s="9" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="U5" s="9"/>
       <c r="V5" s="9"/>
       <c r="W5" s="9"/>
       <c r="X5" s="11" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="Y5" s="11">
         <v>2013</v>
       </c>
       <c r="Z5" s="11" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="AA5" s="11"/>
       <c r="AB5" s="11" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="AC5" s="11" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="AD5" s="11" t="s">
         <v>88</v>
       </c>
       <c r="AE5" s="11"/>
       <c r="AF5" s="11" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="AG5" s="9" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="AH5" s="9" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="AI5" s="9" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="AJ5" s="9" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="AK5" s="9"/>
       <c r="AL5" s="21"/>
     </row>
-    <row r="6" spans="1:38" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" s="2" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>15</v>
       </c>
@@ -1912,20 +1921,22 @@
         <v>7</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="E6" s="10"/>
+        <v>194</v>
+      </c>
+      <c r="D6" s="9">
+        <v>2017</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>206</v>
+      </c>
       <c r="F6" s="9" t="s">
         <v>78</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>171</v>
+        <v>195</v>
       </c>
       <c r="I6" s="11" t="s">
         <v>79</v>
@@ -1942,27 +1953,27 @@
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
       <c r="O6" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P6" s="9">
         <v>2015</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R6" s="9"/>
       <c r="S6" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T6" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U6" s="9" t="s">
         <v>88</v>
       </c>
       <c r="V6" s="9"/>
       <c r="W6" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="X6" s="11"/>
       <c r="Y6" s="11"/>
@@ -1973,19 +1984,19 @@
       <c r="AD6" s="11"/>
       <c r="AE6" s="11"/>
       <c r="AF6" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="AG6" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="AH6" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI6" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="AH6" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="AI6" s="9" t="s">
-        <v>116</v>
-      </c>
       <c r="AJ6" s="9" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="AK6" s="9" t="s">
         <v>69</v>
@@ -2000,20 +2011,22 @@
         <v>9</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="D7" s="9">
-        <v>2010</v>
-      </c>
-      <c r="E7" s="10"/>
+        <v>202</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>207</v>
+      </c>
       <c r="F7" s="9" t="s">
         <v>78</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>79</v>
@@ -2030,39 +2043,43 @@
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
       <c r="O7" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="P7" s="9">
         <v>2017</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R7" s="9"/>
       <c r="S7" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="T7" s="9" t="s">
         <v>135</v>
-      </c>
-      <c r="T7" s="9" t="s">
-        <v>137</v>
       </c>
       <c r="U7" s="9" t="s">
         <v>88</v>
       </c>
       <c r="V7" s="9"/>
       <c r="W7" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="11"/>
-      <c r="Z7" s="11"/>
+        <v>111</v>
+      </c>
+      <c r="X7" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="Y7" s="11">
+        <v>2014</v>
+      </c>
+      <c r="Z7" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="AA7" s="11"/>
       <c r="AB7" s="11"/>
       <c r="AC7" s="11"/>
       <c r="AD7" s="11"/>
       <c r="AE7" s="11"/>
-      <c r="AF7" s="11" t="s">
-        <v>188</v>
-      </c>
+      <c r="AF7" s="11"/>
       <c r="AG7" s="9"/>
       <c r="AH7" s="9"/>
       <c r="AI7" s="9"/>
@@ -2078,20 +2095,22 @@
         <v>10</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="D8" s="9">
-        <v>2010</v>
-      </c>
-      <c r="E8" s="10"/>
+        <v>198</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>208</v>
+      </c>
       <c r="F8" s="9" t="s">
         <v>78</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>79</v>
@@ -2108,50 +2127,50 @@
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
       <c r="O8" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="P8" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q8" s="9" t="s">
         <v>130</v>
-      </c>
-      <c r="Q8" s="9" t="s">
-        <v>132</v>
       </c>
       <c r="R8" s="9"/>
       <c r="S8" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="T8" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U8" s="9" t="s">
         <v>88</v>
       </c>
       <c r="V8" s="9"/>
       <c r="W8" s="9" t="s">
-        <v>131</v>
+        <v>201</v>
       </c>
       <c r="X8" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Y8" s="11">
         <v>2013</v>
       </c>
       <c r="Z8" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AA8" s="11"/>
       <c r="AB8" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AC8" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AD8" s="11" t="s">
         <v>88</v>
       </c>
       <c r="AE8" s="11"/>
       <c r="AF8" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="AG8" s="9"/>
       <c r="AH8" s="9"/>
@@ -2168,20 +2187,22 @@
         <v>11</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>163</v>
+        <v>200</v>
       </c>
       <c r="D9" s="9">
         <v>2017</v>
       </c>
-      <c r="E9" s="10"/>
+      <c r="E9" s="10" t="s">
+        <v>209</v>
+      </c>
       <c r="F9" s="9" t="s">
         <v>78</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="I9" s="11" t="s">
         <v>79</v>
@@ -2198,20 +2219,20 @@
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
       <c r="O9" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="P9" s="9">
         <v>2012</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R9" s="9"/>
       <c r="S9" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="T9" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="U9" s="9" t="s">
         <v>88</v>
@@ -2219,20 +2240,20 @@
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
       <c r="X9" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Y9" s="11">
         <v>2015</v>
       </c>
       <c r="Z9" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AA9" s="11"/>
       <c r="AB9" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AC9" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AD9" s="11" t="s">
         <v>88</v>
@@ -2254,13 +2275,13 @@
         <v>5</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D10" s="9">
         <v>2011</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9" t="s">
@@ -2281,20 +2302,20 @@
       </c>
       <c r="M10" s="11"/>
       <c r="N10" s="11" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="P10" s="9">
         <v>2013</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="R10" s="9"/>
       <c r="S10" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="T10" s="9"/>
       <c r="U10" s="9" t="s">
@@ -2312,13 +2333,13 @@
       <c r="AE10" s="11"/>
       <c r="AF10" s="11"/>
       <c r="AG10" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AH10" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AI10" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="AJ10" s="9"/>
       <c r="AK10" s="9" t="s">
@@ -2334,13 +2355,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D11" s="9">
         <v>2011</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9" t="s">
@@ -2361,20 +2382,20 @@
       </c>
       <c r="M11" s="11"/>
       <c r="N11" s="11" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="P11" s="9">
         <v>2011</v>
       </c>
       <c r="Q11" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="R11" s="9"/>
       <c r="S11" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="T11" s="9"/>
       <c r="U11" s="9" t="s">
@@ -2392,13 +2413,13 @@
       <c r="AE11" s="11"/>
       <c r="AF11" s="11"/>
       <c r="AG11" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="AH11" s="9">
         <v>2011</v>
       </c>
       <c r="AI11" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AJ11" s="9"/>
       <c r="AK11" s="9" t="s">
@@ -2414,13 +2435,13 @@
         <v>18</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D12" s="9">
         <v>2011</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9" t="s">
@@ -2441,7 +2462,7 @@
       </c>
       <c r="M12" s="11"/>
       <c r="N12" s="11" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
@@ -2462,11 +2483,11 @@
       <c r="AE12" s="11"/>
       <c r="AF12" s="11"/>
       <c r="AG12" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AH12" s="9"/>
       <c r="AI12" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="AJ12" s="9"/>
       <c r="AK12" s="9" t="s">
@@ -2476,7 +2497,7 @@
     </row>
     <row r="13" spans="1:38" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B13" s="30"/>
       <c r="C13" s="30"/>
@@ -2554,13 +2575,13 @@
       <c r="AE14" s="11"/>
       <c r="AF14" s="11"/>
       <c r="AG14" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="AH14" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AI14" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AJ14" s="9"/>
       <c r="AK14" s="9"/>
@@ -2568,10 +2589,10 @@
     </row>
     <row r="15" spans="1:38" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -2675,7 +2696,7 @@
     <hyperlink ref="K10" r:id="rId8" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{2DA8DA9C-5C56-4732-B7E0-F0EA32AEBAC8}"/>
     <hyperlink ref="K11" r:id="rId9" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{4DF01CCA-22EB-4871-AAF9-A63A4C27488F}"/>
     <hyperlink ref="K12" r:id="rId10" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{88B17616-30B0-4EEA-9A95-F3420944DE6B}"/>
-    <hyperlink ref="E5" r:id="rId11" xr:uid="{487BE792-960F-4530-BF8E-EAC833016D5D}"/>
+    <hyperlink ref="E5" r:id="rId11" display="https://github.com/ITHIM/ITHIM-R/tree/master/inst/extdata/local/belo_horizonte" xr:uid="{487BE792-960F-4530-BF8E-EAC833016D5D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId12"/>

</xml_diff>

<commit_message>
updated case studies file
</commit_message>
<xml_diff>
--- a/project_mgmt/case_cities_data.xlsx
+++ b/project_mgmt/case_cities_data.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmtg3\OneDrive\Cambridge\TIGTHAT\ITHIM-R\project_mgmt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ITHIM-R\project_mgmt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="211" documentId="13_ncr:1_{58B9BE8B-73DC-4B84-B270-ADD34A1BB702}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{13226F7D-9110-4D89-A4D8-E344B46DA5C8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Data variables" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="210">
   <si>
     <t>Country</t>
   </si>
@@ -448,18 +447,6 @@
     <t>Data exist. Request sent 3 times but no return from authorities.</t>
   </si>
   <si>
-    <t>C:/Users/rg574/Dropbox/Who hit who matrices international/Cities database/England</t>
-  </si>
-  <si>
-    <t>C:/Users/rg574/Dropbox/Who hit who matrices international/Cities database/India/Bengaluru</t>
-  </si>
-  <si>
-    <t>C:/Users/rg574/Dropbox/Who hit who matrices international/Cities database/India/Delhi</t>
-  </si>
-  <si>
-    <t>C:/Users/rg574/Dropbox/Who hit who matrices international/Cities database/India/Fatality_data_Indian cities/visakhapatnam</t>
-  </si>
-  <si>
     <t>Rob Johnson accessed from Anna/STATS19</t>
   </si>
   <si>
@@ -473,9 +460,6 @@
   </si>
   <si>
     <t>2005-2015</t>
-  </si>
-  <si>
-    <t>C:/Users/rg574/Dropbox/Who hit who matrices international/Cities database/Ghana</t>
   </si>
   <si>
     <t>2007-2016</t>
@@ -708,11 +692,23 @@
   <si>
     <t>Study on Global Aging and Adult Health (SAGE) - Wave 2</t>
   </si>
+  <si>
+    <t>Rob Johnson processed this data, which is what is in this folder now</t>
+  </si>
+  <si>
+    <t>V:\Studies\MOVED\HealthImpact\Data\TIGTHAT\Accra\Accra data and microdata\RTI\injury data</t>
+  </si>
+  <si>
+    <t>V:/Studies/MOVED/HealthImpact/Data/TIGTHAT/India/injury data indian cities/Fatality_data_Indian cities/</t>
+  </si>
+  <si>
+    <t>V:/Studies/MOVED/HealthImpact/Data/TIGTHAT/India/injury data indian cities/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1412,14 +1408,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:B1"/>
+      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,7 +1427,7 @@
   <sheetData>
     <row r="1" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="34" t="s">
@@ -1534,7 +1530,7 @@
         <v>35</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="S2" s="5" t="s">
         <v>38</v>
@@ -1546,7 +1542,7 @@
         <v>37</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="W2" s="5" t="s">
         <v>40</v>
@@ -1561,7 +1557,7 @@
         <v>35</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="AB2" s="6" t="s">
         <v>38</v>
@@ -1573,7 +1569,7 @@
         <v>37</v>
       </c>
       <c r="AE2" s="6" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="AF2" s="6" t="s">
         <v>40</v>
@@ -1605,13 +1601,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>78</v>
@@ -1620,7 +1616,7 @@
         <v>69</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="I3" s="16" t="s">
         <v>79</v>
@@ -1683,27 +1679,29 @@
         <v>69</v>
       </c>
       <c r="AE3" s="16" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="AF3" s="16" t="s">
         <v>100</v>
       </c>
       <c r="AG3" s="14" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="AH3" s="14" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="AI3" s="14" t="s">
-        <v>147</v>
+        <v>207</v>
       </c>
       <c r="AJ3" s="14" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="AK3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="AL3" s="19"/>
+      <c r="AL3" s="19" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="4" spans="1:38" s="2" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
@@ -1713,13 +1711,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>78</v>
@@ -1782,19 +1780,19 @@
         <v>3082</v>
       </c>
       <c r="AB4" s="11" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="AC4" s="11" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="AD4" s="11" t="s">
         <v>69</v>
       </c>
       <c r="AE4" s="11" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="AF4" s="11" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="AG4" s="9" t="s">
         <v>105</v>
@@ -1812,7 +1810,7 @@
         <v>69</v>
       </c>
       <c r="AL4" s="21" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:38" s="2" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1820,16 +1818,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>78</v>
@@ -1838,7 +1836,7 @@
         <v>69</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="I5" s="16" t="s">
         <v>79</v>
@@ -1854,7 +1852,7 @@
       </c>
       <c r="M5" s="11"/>
       <c r="N5" s="11" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="O5" s="9" t="s">
         <v>119</v>
@@ -1863,52 +1861,52 @@
         <v>2012</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="R5" s="9"/>
       <c r="S5" s="9" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="T5" s="9" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="U5" s="9"/>
       <c r="V5" s="9"/>
       <c r="W5" s="9"/>
       <c r="X5" s="11" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="Y5" s="11">
         <v>2013</v>
       </c>
       <c r="Z5" s="11" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="AA5" s="11"/>
       <c r="AB5" s="11" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="AC5" s="11" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="AD5" s="11" t="s">
         <v>88</v>
       </c>
       <c r="AE5" s="11"/>
       <c r="AF5" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="AG5" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="AH5" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="AI5" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="AG5" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="AH5" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="AI5" s="9" t="s">
-        <v>193</v>
-      </c>
       <c r="AJ5" s="9" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="AK5" s="9"/>
       <c r="AL5" s="21"/>
@@ -1921,13 +1919,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D6" s="9">
         <v>2017</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>78</v>
@@ -1936,7 +1934,7 @@
         <v>69</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="I6" s="11" t="s">
         <v>79</v>
@@ -1996,7 +1994,7 @@
         <v>115</v>
       </c>
       <c r="AJ6" s="9" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="AK6" s="9" t="s">
         <v>69</v>
@@ -2011,13 +2009,13 @@
         <v>9</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>202</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>207</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>78</v>
@@ -2026,7 +2024,7 @@
         <v>69</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>79</v>
@@ -2066,7 +2064,7 @@
         <v>111</v>
       </c>
       <c r="X7" s="16" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="Y7" s="11">
         <v>2014</v>
@@ -2095,13 +2093,13 @@
         <v>10</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>78</v>
@@ -2110,7 +2108,7 @@
         <v>69</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>79</v>
@@ -2147,7 +2145,7 @@
       </c>
       <c r="V8" s="9"/>
       <c r="W8" s="9" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="X8" s="11" t="s">
         <v>124</v>
@@ -2187,13 +2185,13 @@
         <v>11</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D9" s="9">
         <v>2017</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>78</v>
@@ -2202,7 +2200,7 @@
         <v>69</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="I9" s="11" t="s">
         <v>79</v>
@@ -2267,7 +2265,7 @@
       <c r="AK9" s="9"/>
       <c r="AL9" s="21"/>
     </row>
-    <row r="10" spans="1:38" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>14</v>
       </c>
@@ -2275,13 +2273,13 @@
         <v>5</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D10" s="9">
         <v>2011</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9" t="s">
@@ -2302,20 +2300,20 @@
       </c>
       <c r="M10" s="11"/>
       <c r="N10" s="11" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="P10" s="9">
         <v>2013</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="R10" s="9"/>
       <c r="S10" s="9" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="T10" s="9"/>
       <c r="U10" s="9" t="s">
@@ -2333,13 +2331,13 @@
       <c r="AE10" s="11"/>
       <c r="AF10" s="11"/>
       <c r="AG10" s="9" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="AH10" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="AI10" s="9" t="s">
-        <v>140</v>
+        <v>209</v>
       </c>
       <c r="AJ10" s="9"/>
       <c r="AK10" s="9" t="s">
@@ -2347,7 +2345,7 @@
       </c>
       <c r="AL10" s="21"/>
     </row>
-    <row r="11" spans="1:38" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>14</v>
       </c>
@@ -2355,13 +2353,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D11" s="9">
         <v>2011</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9" t="s">
@@ -2382,20 +2380,20 @@
       </c>
       <c r="M11" s="11"/>
       <c r="N11" s="11" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="P11" s="9">
         <v>2011</v>
       </c>
       <c r="Q11" s="9" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="R11" s="9"/>
       <c r="S11" s="9" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="T11" s="9"/>
       <c r="U11" s="9" t="s">
@@ -2413,13 +2411,13 @@
       <c r="AE11" s="11"/>
       <c r="AF11" s="11"/>
       <c r="AG11" s="9" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="AH11" s="9">
         <v>2011</v>
       </c>
       <c r="AI11" s="9" t="s">
-        <v>139</v>
+        <v>208</v>
       </c>
       <c r="AJ11" s="9"/>
       <c r="AK11" s="9" t="s">
@@ -2427,7 +2425,7 @@
       </c>
       <c r="AL11" s="21"/>
     </row>
-    <row r="12" spans="1:38" s="2" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>14</v>
       </c>
@@ -2435,13 +2433,13 @@
         <v>18</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D12" s="9">
         <v>2011</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9" t="s">
@@ -2462,7 +2460,7 @@
       </c>
       <c r="M12" s="11"/>
       <c r="N12" s="11" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
@@ -2483,11 +2481,11 @@
       <c r="AE12" s="11"/>
       <c r="AF12" s="11"/>
       <c r="AG12" s="9" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="AH12" s="9"/>
       <c r="AI12" s="9" t="s">
-        <v>141</v>
+        <v>208</v>
       </c>
       <c r="AJ12" s="9"/>
       <c r="AK12" s="9" t="s">
@@ -2497,7 +2495,7 @@
     </row>
     <row r="13" spans="1:38" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B13" s="30"/>
       <c r="C13" s="30"/>
@@ -2537,7 +2535,7 @@
       <c r="AK13" s="30"/>
       <c r="AL13" s="31"/>
     </row>
-    <row r="14" spans="1:38" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>16</v>
       </c>
@@ -2575,24 +2573,22 @@
       <c r="AE14" s="11"/>
       <c r="AF14" s="11"/>
       <c r="AG14" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="AH14" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="AH14" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI14" s="9" t="s">
-        <v>138</v>
-      </c>
+      <c r="AI14" s="9"/>
       <c r="AJ14" s="9"/>
       <c r="AK14" s="9"/>
       <c r="AL14" s="21"/>
     </row>
     <row r="15" spans="1:38" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -2631,7 +2627,7 @@
       <c r="AK15" s="9"/>
       <c r="AL15" s="21"/>
     </row>
-    <row r="16" spans="1:38" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>21</v>
       </c>
@@ -2686,17 +2682,17 @@
     <mergeCell ref="C1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="K4" r:id="rId2" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="K6" r:id="rId3" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="K7" r:id="rId4" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="K8" r:id="rId5" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="K9" r:id="rId6" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="K5" r:id="rId7" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{BCDDC5AF-6E28-4005-8C24-7B6A8AA12123}"/>
-    <hyperlink ref="K10" r:id="rId8" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{2DA8DA9C-5C56-4732-B7E0-F0EA32AEBAC8}"/>
-    <hyperlink ref="K11" r:id="rId9" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{4DF01CCA-22EB-4871-AAF9-A63A4C27488F}"/>
-    <hyperlink ref="K12" r:id="rId10" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{88B17616-30B0-4EEA-9A95-F3420944DE6B}"/>
-    <hyperlink ref="E5" r:id="rId11" display="https://github.com/ITHIM/ITHIM-R/tree/master/inst/extdata/local/belo_horizonte" xr:uid="{487BE792-960F-4530-BF8E-EAC833016D5D}"/>
+    <hyperlink ref="K3" r:id="rId1" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv"/>
+    <hyperlink ref="K4" r:id="rId2" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv"/>
+    <hyperlink ref="K6" r:id="rId3" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv"/>
+    <hyperlink ref="K7" r:id="rId4" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv"/>
+    <hyperlink ref="K8" r:id="rId5" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv"/>
+    <hyperlink ref="K9" r:id="rId6" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv"/>
+    <hyperlink ref="K5" r:id="rId7" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv"/>
+    <hyperlink ref="K10" r:id="rId8" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv"/>
+    <hyperlink ref="K11" r:id="rId9" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv"/>
+    <hyperlink ref="K12" r:id="rId10" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv"/>
+    <hyperlink ref="E5" r:id="rId11" display="https://github.com/ITHIM/ITHIM-R/tree/master/inst/extdata/local/belo_horizonte"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId12"/>
@@ -2704,7 +2700,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Updated Indian cities PA data
</commit_message>
<xml_diff>
--- a/project_mgmt/case_cities_data.xlsx
+++ b/project_mgmt/case_cities_data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ITHIM-R\project_mgmt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmtg3\OneDrive\Cambridge\TIGTHAT\ITHIM-R\project_mgmt\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_E002D655F0BF92CA70A528B0D98F24444305BC0C" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{0CD5E0F0-CFF8-4EB9-A735-EAFD53428D90}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -20,18 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="211">
   <si>
     <t>Country</t>
   </si>
@@ -704,11 +699,14 @@
   <si>
     <t>V:/Studies/MOVED/HealthImpact/Data/TIGTHAT/India/injury data indian cities/</t>
   </si>
+  <si>
+    <t>V:\Studies\MOVED\HealthImpact\Data\TIGTHAT\India\SAGE data 2007</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1408,14 +1406,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="T6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2265,7 +2263,7 @@
       <c r="AK9" s="9"/>
       <c r="AL9" s="21"/>
     </row>
-    <row r="10" spans="1:38" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" s="2" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>14</v>
       </c>
@@ -2321,13 +2319,25 @@
       </c>
       <c r="V10" s="9"/>
       <c r="W10" s="9"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="11"/>
-      <c r="AA10" s="11"/>
-      <c r="AB10" s="11"/>
-      <c r="AC10" s="11"/>
-      <c r="AD10" s="11"/>
+      <c r="X10" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y10" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z10" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA10" s="16"/>
+      <c r="AB10" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="AC10" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD10" s="16" t="s">
+        <v>88</v>
+      </c>
       <c r="AE10" s="11"/>
       <c r="AF10" s="11"/>
       <c r="AG10" s="9" t="s">
@@ -2345,7 +2355,7 @@
       </c>
       <c r="AL10" s="21"/>
     </row>
-    <row r="11" spans="1:38" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" s="2" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>14</v>
       </c>
@@ -2401,13 +2411,25 @@
       </c>
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="11"/>
-      <c r="Z11" s="11"/>
-      <c r="AA11" s="11"/>
-      <c r="AB11" s="11"/>
-      <c r="AC11" s="11"/>
-      <c r="AD11" s="11"/>
+      <c r="X11" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y11" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z11" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA11" s="16"/>
+      <c r="AB11" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="AC11" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD11" s="16" t="s">
+        <v>88</v>
+      </c>
       <c r="AE11" s="11"/>
       <c r="AF11" s="11"/>
       <c r="AG11" s="9" t="s">
@@ -2471,13 +2493,25 @@
       <c r="U12" s="9"/>
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
-      <c r="X12" s="11"/>
-      <c r="Y12" s="11"/>
-      <c r="Z12" s="11"/>
-      <c r="AA12" s="11"/>
-      <c r="AB12" s="11"/>
-      <c r="AC12" s="11"/>
-      <c r="AD12" s="11"/>
+      <c r="X12" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y12" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z12" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA12" s="16"/>
+      <c r="AB12" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="AC12" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD12" s="16" t="s">
+        <v>88</v>
+      </c>
       <c r="AE12" s="11"/>
       <c r="AF12" s="11"/>
       <c r="AG12" s="9" t="s">
@@ -2627,7 +2661,7 @@
       <c r="AK15" s="9"/>
       <c r="AL15" s="21"/>
     </row>
-    <row r="16" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>21</v>
       </c>
@@ -2682,17 +2716,17 @@
     <mergeCell ref="C1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv"/>
-    <hyperlink ref="K4" r:id="rId2" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv"/>
-    <hyperlink ref="K6" r:id="rId3" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv"/>
-    <hyperlink ref="K7" r:id="rId4" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv"/>
-    <hyperlink ref="K8" r:id="rId5" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv"/>
-    <hyperlink ref="K9" r:id="rId6" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv"/>
-    <hyperlink ref="K5" r:id="rId7" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv"/>
-    <hyperlink ref="K10" r:id="rId8" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv"/>
-    <hyperlink ref="K11" r:id="rId9" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv"/>
-    <hyperlink ref="K12" r:id="rId10" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv"/>
-    <hyperlink ref="E5" r:id="rId11" display="https://github.com/ITHIM/ITHIM-R/tree/master/inst/extdata/local/belo_horizonte"/>
+    <hyperlink ref="K3" r:id="rId1" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K4" r:id="rId2" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="K6" r:id="rId3" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="K7" r:id="rId4" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="K8" r:id="rId5" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="K9" r:id="rId6" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="K5" r:id="rId7" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="K10" r:id="rId8" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="K11" r:id="rId9" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="K12" r:id="rId10" display="https://github.com/ITHIM/ITHIM-R/blob/master/data/local/accra/gbd_accra.csv" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E5" r:id="rId11" display="https://github.com/ITHIM/ITHIM-R/tree/master/inst/extdata/local/belo_horizonte" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId12"/>
@@ -2700,7 +2734,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Minor updates in the case cities data form.
</commit_message>
<xml_diff>
--- a/project_mgmt/case_cities_data.xlsx
+++ b/project_mgmt/case_cities_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmtg3\OneDrive\Cambridge\TIGTHAT\ITHIM-R\project_mgmt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_E002D655F0BF92CA70A528B0D98F24444305BC0C" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{0CD5E0F0-CFF8-4EB9-A735-EAFD53428D90}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_E002D655F0BF92CA70A528B0D98F24444305BC0C" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{E98B1A18-FD70-47E7-834A-7CAD30BEEF35}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="207">
   <si>
     <t>Country</t>
   </si>
@@ -325,15 +325,9 @@
     <t>University of Sao Paulo School of Public Health</t>
   </si>
   <si>
-    <t>Datasets on household and individual characteristics also available in the same folder. Dataset must be filter in for urban Greater Accra region.</t>
-  </si>
-  <si>
     <t>Datasets on household and individual characteristics also available in the same folder (compressed folder 'Datasets'). Dataset must be filter in for urban Greater Accra region.</t>
   </si>
   <si>
-    <t>Covers Sao Paulo Metropolitan Area.</t>
-  </si>
-  <si>
     <t>2011-2015</t>
   </si>
   <si>
@@ -361,9 +355,6 @@
     <t>V:\Studies\MOVED\HealthImpact\Data\TIGTHAT\Colombia\Bogota\Travel</t>
   </si>
   <si>
-    <t>Multiple files.</t>
-  </si>
-  <si>
     <t>2010-2017</t>
   </si>
   <si>
@@ -482,9 +473,6 @@
   </si>
   <si>
     <t>Our area is Valley of Mexico Metropolitan Area, formed by 61 cities: Acolman, Amecameca, Apaxco, Atenco, Atizapán de Zaragoza, Atlautla, Axapusco, Ayapango, Chalco, Chiautla, Chicoloapan, Chiconcuac, Chimalhuacán, Coacalco de Berriozábal, Cocotitlán, Coyotepec, Cuautitlán, Cuautitlán Izcalli, Ecatepec de Morelos, Ecatzingo, Huehuetoca, Hueypoxtla, Huixquilucan, Isidro Fabela, Ixtapaluca, Jaltenco, Jilotzingo, Juchitepec, La Paz, Melchor Ocampo, Mexico City, Naucalpan de Juárez, Nextlalpan, Nezahualcóyotl, Nicolás Romero, Nopaltepec, Otumba, Ozumba, Papalotla, San Martín de las Pirámides, Tecámac, Temamatla, Temascalapa, Tenango del Aire, Teoloyucan, Teotihuacán, Tepetlaoxtoc, Tepetlixpa, Tepotzotlán, Tequixquiac, Texcoco, Tezoyuca, Tizayuca, Tlalmanalco, Tlalnepantla de Baz, Tonanitla, Tultepec, Tultitlán, Valle de Chalco Solidaridad, Villa del Carbón, Zumpango.</t>
-  </si>
-  <si>
-    <t>Our area is Greater Accra Metropolitan Area, formed by 12 districts: Accra Metropolitan District, Tema Metropolis, Adenta, Ga East, Ga West, Ga South, Ga Central, La Nkwantang-Madina, Ledzokuku-Krowor, Ashaiman, Kpone-Katamanso, La Dade-Kotopon.</t>
   </si>
   <si>
     <t>Our area is Santiago Metropolitan Area, formed by 52 cities:  Alhué, Buin, Calera de Tango, Cerrillos, Cerro Navia, Colina, Conchalí, Curacaví, El Bosque, El Monte, Estación Central, Huechuraba, Independencia, Isla de Maipo, La Cisterna, La Florida, La Granja, La Pintana, La Reina, Lampa, Las Condes, Lo Barnechea, Lo Espejo, Lo Prado, Macul, Maipú, María Pinto, Melipilla, Ñuñoa, Padre Hurtado, Paine, Pedro Aguirre Cerda, Peñaflor, Peñalolén, Pirque, Providencia, Pudahuel, Puente Alto, Quilicura, Quinta Normal, Recoleta, Renca, San Bernardo, San Joaquín, San José de Maipo, San Miguel, San Pedro, San Ramón, Santiago, Talagante, Til Til, Vitacura</t>
@@ -658,9 +646,6 @@
     <t>Chile Population and Housing Census</t>
   </si>
   <si>
-    <t>Multiple files. Buenos Aires Metropolitan Area (larger than Gran Buenos Aires).</t>
-  </si>
-  <si>
     <t>Mexico Population and Housing Census (2010) &amp; population projection (2017)</t>
   </si>
   <si>
@@ -701,6 +686,9 @@
   </si>
   <si>
     <t>V:\Studies\MOVED\HealthImpact\Data\TIGTHAT\India\SAGE data 2007</t>
+  </si>
+  <si>
+    <t>Our area is Greater Accra Metropolitan Area, formed by 12 districts: Accra Metropolitan District, Tema Metropolis, Adenta, Ga East, Ga West, Ga South, Ga Central, La Nkwantang-Madina, Ledzokuku-Krowor, Ashaiman, Kpone-Katamanso, La Dade-Kotopon. Dataset must be filter in for urban Greater Accra region.</t>
   </si>
 </sst>
 </file>
@@ -1409,11 +1397,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="T6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X10" sqref="X10"/>
+      <selection pane="bottomRight" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,7 +1413,7 @@
   <sheetData>
     <row r="1" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="34" t="s">
@@ -1528,7 +1516,7 @@
         <v>35</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="S2" s="5" t="s">
         <v>38</v>
@@ -1540,7 +1528,7 @@
         <v>37</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="W2" s="5" t="s">
         <v>40</v>
@@ -1555,7 +1543,7 @@
         <v>35</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AB2" s="6" t="s">
         <v>38</v>
@@ -1567,7 +1555,7 @@
         <v>37</v>
       </c>
       <c r="AE2" s="6" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="AF2" s="6" t="s">
         <v>40</v>
@@ -1599,13 +1587,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>78</v>
@@ -1613,9 +1601,7 @@
       <c r="G3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="14" t="s">
-        <v>152</v>
-      </c>
+      <c r="H3" s="14"/>
       <c r="I3" s="16" t="s">
         <v>79</v>
       </c>
@@ -1646,14 +1632,14 @@
         <v>70</v>
       </c>
       <c r="T3" s="14" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="U3" s="14" t="s">
         <v>69</v>
       </c>
       <c r="V3" s="14"/>
       <c r="W3" s="14" t="s">
-        <v>99</v>
+        <v>206</v>
       </c>
       <c r="X3" s="16" t="s">
         <v>72</v>
@@ -1671,34 +1657,34 @@
         <v>76</v>
       </c>
       <c r="AC3" s="16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AD3" s="16" t="s">
         <v>69</v>
       </c>
       <c r="AE3" s="16" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="AF3" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AG3" s="14" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="AH3" s="14" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="AI3" s="14" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="AJ3" s="14" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="AK3" s="14" t="s">
         <v>69</v>
       </c>
       <c r="AL3" s="19" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:38" s="2" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1709,13 +1695,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>78</v>
@@ -1723,9 +1709,7 @@
       <c r="G4" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>106</v>
-      </c>
+      <c r="H4" s="9"/>
       <c r="I4" s="11" t="s">
         <v>79</v>
       </c>
@@ -1740,7 +1724,7 @@
       </c>
       <c r="M4" s="11"/>
       <c r="N4" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O4" s="9" t="s">
         <v>93</v>
@@ -1763,7 +1747,7 @@
       </c>
       <c r="V4" s="9"/>
       <c r="W4" s="9" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="X4" s="11" t="s">
         <v>97</v>
@@ -1778,37 +1762,37 @@
         <v>3082</v>
       </c>
       <c r="AB4" s="11" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="AC4" s="11" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="AD4" s="11" t="s">
         <v>69</v>
       </c>
       <c r="AE4" s="11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="AF4" s="11" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="AG4" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="AH4" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI4" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AJ4" s="9" t="s">
         <v>102</v>
-      </c>
-      <c r="AI4" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="AJ4" s="9" t="s">
-        <v>104</v>
       </c>
       <c r="AK4" s="9" t="s">
         <v>69</v>
       </c>
       <c r="AL4" s="21" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:38" s="2" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1816,16 +1800,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>78</v>
@@ -1833,9 +1817,7 @@
       <c r="G5" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>174</v>
-      </c>
+      <c r="H5" s="9"/>
       <c r="I5" s="16" t="s">
         <v>79</v>
       </c>
@@ -1850,61 +1832,63 @@
       </c>
       <c r="M5" s="11"/>
       <c r="N5" s="11" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="P5" s="9">
         <v>2012</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="R5" s="9"/>
       <c r="S5" s="9" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="T5" s="9" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="U5" s="9"/>
       <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
+      <c r="W5" s="9" t="s">
+        <v>170</v>
+      </c>
       <c r="X5" s="11" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="Y5" s="11">
         <v>2013</v>
       </c>
       <c r="Z5" s="11" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="AA5" s="11"/>
       <c r="AB5" s="11" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="AC5" s="11" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="AD5" s="11" t="s">
         <v>88</v>
       </c>
       <c r="AE5" s="11"/>
       <c r="AF5" s="11" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="AG5" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="AH5" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI5" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="AH5" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="AI5" s="9" t="s">
-        <v>188</v>
-      </c>
       <c r="AJ5" s="9" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="AK5" s="9"/>
       <c r="AL5" s="21"/>
@@ -1917,13 +1901,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D6" s="9">
         <v>2017</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>78</v>
@@ -1931,9 +1915,7 @@
       <c r="G6" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>190</v>
-      </c>
+      <c r="H6" s="9"/>
       <c r="I6" s="11" t="s">
         <v>79</v>
       </c>
@@ -1955,21 +1937,21 @@
         <v>2015</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R6" s="9"/>
       <c r="S6" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="T6" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="U6" s="9" t="s">
         <v>88</v>
       </c>
       <c r="V6" s="9"/>
       <c r="W6" s="9" t="s">
-        <v>111</v>
+        <v>186</v>
       </c>
       <c r="X6" s="11"/>
       <c r="Y6" s="11"/>
@@ -1980,19 +1962,19 @@
       <c r="AD6" s="11"/>
       <c r="AE6" s="11"/>
       <c r="AF6" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="AG6" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="AH6" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI6" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="AI6" s="9" t="s">
-        <v>115</v>
-      </c>
       <c r="AJ6" s="9" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="AK6" s="9" t="s">
         <v>69</v>
@@ -2007,13 +1989,13 @@
         <v>9</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>197</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>202</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>78</v>
@@ -2021,9 +2003,7 @@
       <c r="G7" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H7" s="9" t="s">
-        <v>151</v>
-      </c>
+      <c r="H7" s="9"/>
       <c r="I7" s="11" t="s">
         <v>79</v>
       </c>
@@ -2039,30 +2019,30 @@
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
       <c r="O7" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="P7" s="9">
         <v>2017</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R7" s="9"/>
       <c r="S7" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="T7" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="U7" s="9" t="s">
         <v>88</v>
       </c>
       <c r="V7" s="9"/>
       <c r="W7" s="9" t="s">
-        <v>111</v>
+        <v>148</v>
       </c>
       <c r="X7" s="16" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="Y7" s="11">
         <v>2014</v>
@@ -2091,13 +2071,13 @@
         <v>10</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>78</v>
@@ -2105,9 +2085,7 @@
       <c r="G8" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>194</v>
-      </c>
+      <c r="H8" s="9"/>
       <c r="I8" s="11" t="s">
         <v>79</v>
       </c>
@@ -2123,50 +2101,50 @@
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
       <c r="O8" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="R8" s="9"/>
       <c r="S8" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="T8" s="9" t="s">
         <v>128</v>
-      </c>
-      <c r="T8" s="9" t="s">
-        <v>131</v>
       </c>
       <c r="U8" s="9" t="s">
         <v>88</v>
       </c>
       <c r="V8" s="9"/>
       <c r="W8" s="9" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="X8" s="11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="Y8" s="11">
         <v>2013</v>
       </c>
       <c r="Z8" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="AA8" s="11"/>
       <c r="AB8" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="AC8" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="AD8" s="11" t="s">
         <v>88</v>
       </c>
       <c r="AE8" s="11"/>
       <c r="AF8" s="11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AG8" s="9"/>
       <c r="AH8" s="9"/>
@@ -2183,13 +2161,13 @@
         <v>11</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D9" s="9">
         <v>2017</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>78</v>
@@ -2197,9 +2175,7 @@
       <c r="G9" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>153</v>
-      </c>
+      <c r="H9" s="9"/>
       <c r="I9" s="11" t="s">
         <v>79</v>
       </c>
@@ -2215,41 +2191,43 @@
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
       <c r="O9" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="P9" s="9">
         <v>2012</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="R9" s="9"/>
       <c r="S9" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="T9" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="U9" s="9" t="s">
         <v>88</v>
       </c>
       <c r="V9" s="9"/>
-      <c r="W9" s="9"/>
+      <c r="W9" s="9" t="s">
+        <v>149</v>
+      </c>
       <c r="X9" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="Y9" s="11">
         <v>2015</v>
       </c>
       <c r="Z9" s="11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="AA9" s="11"/>
       <c r="AB9" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AC9" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="AD9" s="11" t="s">
         <v>88</v>
@@ -2271,13 +2249,13 @@
         <v>5</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D10" s="9">
         <v>2011</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9" t="s">
@@ -2298,20 +2276,20 @@
       </c>
       <c r="M10" s="11"/>
       <c r="N10" s="11" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="P10" s="9">
         <v>2013</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="R10" s="9"/>
       <c r="S10" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="T10" s="9"/>
       <c r="U10" s="9" t="s">
@@ -2330,10 +2308,10 @@
       </c>
       <c r="AA10" s="16"/>
       <c r="AB10" s="16" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="AC10" s="16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AD10" s="16" t="s">
         <v>88</v>
@@ -2341,13 +2319,13 @@
       <c r="AE10" s="11"/>
       <c r="AF10" s="11"/>
       <c r="AG10" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AH10" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="AI10" s="9" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="AJ10" s="9"/>
       <c r="AK10" s="9" t="s">
@@ -2363,13 +2341,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D11" s="9">
         <v>2011</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9" t="s">
@@ -2390,20 +2368,20 @@
       </c>
       <c r="M11" s="11"/>
       <c r="N11" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="P11" s="9">
         <v>2011</v>
       </c>
       <c r="Q11" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="R11" s="9"/>
       <c r="S11" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="T11" s="9"/>
       <c r="U11" s="9" t="s">
@@ -2422,10 +2400,10 @@
       </c>
       <c r="AA11" s="16"/>
       <c r="AB11" s="16" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="AC11" s="16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AD11" s="16" t="s">
         <v>88</v>
@@ -2433,13 +2411,13 @@
       <c r="AE11" s="11"/>
       <c r="AF11" s="11"/>
       <c r="AG11" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="AH11" s="9">
         <v>2011</v>
       </c>
       <c r="AI11" s="9" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="AJ11" s="9"/>
       <c r="AK11" s="9" t="s">
@@ -2455,13 +2433,13 @@
         <v>18</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D12" s="9">
         <v>2011</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9" t="s">
@@ -2482,7 +2460,7 @@
       </c>
       <c r="M12" s="11"/>
       <c r="N12" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
@@ -2504,10 +2482,10 @@
       </c>
       <c r="AA12" s="16"/>
       <c r="AB12" s="16" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="AC12" s="16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AD12" s="16" t="s">
         <v>88</v>
@@ -2515,11 +2493,11 @@
       <c r="AE12" s="11"/>
       <c r="AF12" s="11"/>
       <c r="AG12" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AH12" s="9"/>
       <c r="AI12" s="9" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="AJ12" s="9"/>
       <c r="AK12" s="9" t="s">
@@ -2529,7 +2507,7 @@
     </row>
     <row r="13" spans="1:38" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B13" s="30"/>
       <c r="C13" s="30"/>
@@ -2607,10 +2585,10 @@
       <c r="AE14" s="11"/>
       <c r="AF14" s="11"/>
       <c r="AG14" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="AH14" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="AI14" s="9"/>
       <c r="AJ14" s="9"/>
@@ -2619,10 +2597,10 @@
     </row>
     <row r="15" spans="1:38" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>

</xml_diff>

<commit_message>
Updated cities data form
</commit_message>
<xml_diff>
--- a/project_mgmt/case_cities_data.xlsx
+++ b/project_mgmt/case_cities_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmtg3\OneDrive\Cambridge\TIGTHAT\ITHIM-R\project_mgmt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_E002D655F0BF92CA70A528B0D98F24444305BC0C" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{E98B1A18-FD70-47E7-834A-7CAD30BEEF35}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="11_E002D655F0BF92CA70A528B0D98F24444305BC0C" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{1FFC166F-0958-4D94-971C-186FC78D4F22}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="208">
   <si>
     <t>Country</t>
   </si>
@@ -325,9 +325,6 @@
     <t>University of Sao Paulo School of Public Health</t>
   </si>
   <si>
-    <t>Datasets on household and individual characteristics also available in the same folder (compressed folder 'Datasets'). Dataset must be filter in for urban Greater Accra region.</t>
-  </si>
-  <si>
     <t>2011-2015</t>
   </si>
   <si>
@@ -425,12 +422,6 @@
   </si>
   <si>
     <t>Openly available (http://www.beta.inegi.org.mx/programas/eod/2017/)</t>
-  </si>
-  <si>
-    <t>Data dictionary in the same folder (doc_base_usuario_enfr2013).</t>
-  </si>
-  <si>
-    <t>Data exist. Request sent 3 times but no return from authorities.</t>
   </si>
   <si>
     <t>Rob Johnson accessed from Anna/STATS19</t>
@@ -580,9 +571,6 @@
     <t>2010 &amp; 2017</t>
   </si>
   <si>
-    <t>Our area is Sao Paulo Metropolitan Area, formed by 34 cities: Baldim, Belo Horizonte, Betim, Brumadinho, Caeté, Capim Branco, Confins, Contagem, Esmeraldas, Florestal, Ibirité, Igarapé, Itaguara, Itatiaiuçu, Jaboticatubas, Nova União, Juatuba, Lagoa Santa, Mário Campos, Mateus Leme, Matozinhos, Nova Lima, Pedro Leopoldo, Raposos, Ribeirão das Neves, Rio Acima, Rio Manso, Sabará, Santa Luzia, São Joaquim de Bicas, São José da Lapa, Sarzedo, Taquaraçu de Minas, Vespasiano</t>
-  </si>
-  <si>
     <t>Development Agency of the Belo Horizonte Metropolitan Area</t>
   </si>
   <si>
@@ -604,12 +592,6 @@
     <t>V:\Studies\MOVED\HealthImpact\Data\TIGTHAT\Brazil\Belo Horizonte\Physical activity\Data\PESPNS2013.txt</t>
   </si>
   <si>
-    <t>IPAQ long version. Covers Sao Paulo city only. Data from the 2013 National Health Survey available for the mtropolitan area</t>
-  </si>
-  <si>
-    <t>Covers Belo Horizonte Metropolitan Area</t>
-  </si>
-  <si>
     <t>Mortality surveillance system</t>
   </si>
   <si>
@@ -689,6 +671,27 @@
   </si>
   <si>
     <t>Our area is Greater Accra Metropolitan Area, formed by 12 districts: Accra Metropolitan District, Tema Metropolis, Adenta, Ga East, Ga West, Ga South, Ga Central, La Nkwantang-Madina, Ledzokuku-Krowor, Ashaiman, Kpone-Katamanso, La Dade-Kotopon. Dataset must be filter in for urban Greater Accra region.</t>
+  </si>
+  <si>
+    <t>Our area is Belo Horizonte Metropolitan Area, formed by 34 cities: Baldim, Belo Horizonte, Betim, Brumadinho, Caeté, Capim Branco, Confins, Contagem, Esmeraldas, Florestal, Ibirité, Igarapé, Itaguara, Itatiaiuçu, Jaboticatubas, Nova União, Juatuba, Lagoa Santa, Mário Campos, Mateus Leme, Matozinhos, Nova Lima, Pedro Leopoldo, Raposos, Ribeirão das Neves, Rio Acima, Rio Manso, Sabará, Santa Luzia, São Joaquim de Bicas, São José da Lapa, Sarzedo, Taquaraçu de Minas, Vespasiano</t>
+  </si>
+  <si>
+    <t>National Diet and Nutrition Survey</t>
+  </si>
+  <si>
+    <t>Ministry of Health</t>
+  </si>
+  <si>
+    <t>Available under request to Ministry. Dataset cannot be redistributed. A version of the final paper should be sent to the Ministry.</t>
+  </si>
+  <si>
+    <t>V:\Studies\MOVED\HealthImpact\Data\TIGTHAT\Colombia\Bogota\Physical activity\base-ensin-2015-publica\Formato_Stata\AF_ADULTOS.dta</t>
+  </si>
+  <si>
+    <t>IPAQ long version. Covers Sao Paulo city only. Data from the 2013 National Health Survey (same as Belo Horizonte) also available for the metropolitan area</t>
+  </si>
+  <si>
+    <t>V:\Studies\MOVED\HealthImpact\Data\TIGTHAT\Mexico\Physical activity\MexicoINDDataW2.dta</t>
   </si>
 </sst>
 </file>
@@ -1413,7 +1416,7 @@
   <sheetData>
     <row r="1" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="34" t="s">
@@ -1516,7 +1519,7 @@
         <v>35</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="S2" s="5" t="s">
         <v>38</v>
@@ -1528,7 +1531,7 @@
         <v>37</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="W2" s="5" t="s">
         <v>40</v>
@@ -1543,7 +1546,7 @@
         <v>35</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="AB2" s="6" t="s">
         <v>38</v>
@@ -1555,7 +1558,7 @@
         <v>37</v>
       </c>
       <c r="AE2" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AF2" s="6" t="s">
         <v>40</v>
@@ -1587,13 +1590,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>187</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>193</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>78</v>
@@ -1632,14 +1635,14 @@
         <v>70</v>
       </c>
       <c r="T3" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="U3" s="14" t="s">
         <v>69</v>
       </c>
       <c r="V3" s="14"/>
       <c r="W3" s="14" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="X3" s="16" t="s">
         <v>72</v>
@@ -1657,34 +1660,32 @@
         <v>76</v>
       </c>
       <c r="AC3" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AD3" s="16" t="s">
         <v>69</v>
       </c>
       <c r="AE3" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="AF3" s="16" t="s">
-        <v>99</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="AF3" s="16"/>
       <c r="AG3" s="14" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="AH3" s="14" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AI3" s="14" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="AJ3" s="14" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="AK3" s="14" t="s">
         <v>69</v>
       </c>
       <c r="AL3" s="19" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:38" s="2" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1695,13 +1696,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>188</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>194</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>78</v>
@@ -1724,7 +1725,7 @@
       </c>
       <c r="M4" s="11"/>
       <c r="N4" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O4" s="9" t="s">
         <v>93</v>
@@ -1747,7 +1748,7 @@
       </c>
       <c r="V4" s="9"/>
       <c r="W4" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="X4" s="11" t="s">
         <v>97</v>
@@ -1762,37 +1763,37 @@
         <v>3082</v>
       </c>
       <c r="AB4" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="AC4" s="11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="AD4" s="11" t="s">
         <v>69</v>
       </c>
       <c r="AE4" s="11" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="AF4" s="11" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
       <c r="AG4" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AH4" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI4" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="AI4" s="9" t="s">
+      <c r="AJ4" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="AJ4" s="9" t="s">
-        <v>102</v>
       </c>
       <c r="AK4" s="9" t="s">
         <v>69</v>
       </c>
       <c r="AL4" s="21" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:38" s="2" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1800,16 +1801,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>78</v>
@@ -1832,63 +1833,61 @@
       </c>
       <c r="M5" s="11"/>
       <c r="N5" s="11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P5" s="9">
         <v>2012</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="R5" s="9"/>
       <c r="S5" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="T5" s="9" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="U5" s="9"/>
       <c r="V5" s="9"/>
       <c r="W5" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="X5" s="11" t="s">
         <v>170</v>
-      </c>
-      <c r="X5" s="11" t="s">
-        <v>174</v>
       </c>
       <c r="Y5" s="11">
         <v>2013</v>
       </c>
       <c r="Z5" s="11" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="AA5" s="11"/>
       <c r="AB5" s="11" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AC5" s="11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="AD5" s="11" t="s">
         <v>88</v>
       </c>
       <c r="AE5" s="11"/>
-      <c r="AF5" s="11" t="s">
-        <v>179</v>
-      </c>
+      <c r="AF5" s="11"/>
       <c r="AG5" s="9" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="AH5" s="9" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="AI5" s="9" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="AJ5" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="AK5" s="9"/>
       <c r="AL5" s="21"/>
@@ -1901,13 +1900,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D6" s="9">
         <v>2017</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>78</v>
@@ -1937,44 +1936,54 @@
         <v>2015</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R6" s="9"/>
       <c r="S6" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T6" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="U6" s="9" t="s">
         <v>88</v>
       </c>
       <c r="V6" s="9"/>
       <c r="W6" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
+        <v>180</v>
+      </c>
+      <c r="X6" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y6" s="11">
+        <v>2015</v>
+      </c>
+      <c r="Z6" s="11" t="s">
+        <v>203</v>
+      </c>
       <c r="AA6" s="11"/>
-      <c r="AB6" s="11"/>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="11"/>
+      <c r="AB6" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="AC6" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="AD6" s="11" t="s">
+        <v>88</v>
+      </c>
       <c r="AE6" s="11"/>
-      <c r="AF6" s="11" t="s">
-        <v>134</v>
-      </c>
+      <c r="AF6" s="11"/>
       <c r="AG6" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="AH6" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI6" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="AH6" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="AI6" s="9" t="s">
-        <v>112</v>
-      </c>
       <c r="AJ6" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AK6" s="9" t="s">
         <v>69</v>
@@ -1989,13 +1998,13 @@
         <v>9</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>78</v>
@@ -2019,30 +2028,30 @@
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
       <c r="O7" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P7" s="9">
         <v>2017</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R7" s="9"/>
       <c r="S7" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T7" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U7" s="9" t="s">
         <v>88</v>
       </c>
       <c r="V7" s="9"/>
       <c r="W7" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="X7" s="16" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="Y7" s="11">
         <v>2014</v>
@@ -2051,9 +2060,15 @@
         <v>74</v>
       </c>
       <c r="AA7" s="11"/>
-      <c r="AB7" s="11"/>
-      <c r="AC7" s="11"/>
-      <c r="AD7" s="11"/>
+      <c r="AB7" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="AC7" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD7" s="11" t="s">
+        <v>88</v>
+      </c>
       <c r="AE7" s="11"/>
       <c r="AF7" s="11"/>
       <c r="AG7" s="9"/>
@@ -2071,13 +2086,13 @@
         <v>10</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>78</v>
@@ -2101,51 +2116,49 @@
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
       <c r="O8" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P8" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q8" s="9" t="s">
         <v>126</v>
-      </c>
-      <c r="Q8" s="9" t="s">
-        <v>127</v>
       </c>
       <c r="R8" s="9"/>
       <c r="S8" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T8" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U8" s="9" t="s">
         <v>88</v>
       </c>
       <c r="V8" s="9"/>
       <c r="W8" s="9" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="X8" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Y8" s="11">
         <v>2013</v>
       </c>
       <c r="Z8" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AA8" s="11"/>
       <c r="AB8" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AC8" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AD8" s="11" t="s">
         <v>88</v>
       </c>
       <c r="AE8" s="11"/>
-      <c r="AF8" s="11" t="s">
-        <v>133</v>
-      </c>
+      <c r="AF8" s="11"/>
       <c r="AG8" s="9"/>
       <c r="AH8" s="9"/>
       <c r="AI8" s="9"/>
@@ -2161,13 +2174,13 @@
         <v>11</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D9" s="9">
         <v>2017</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>78</v>
@@ -2191,43 +2204,43 @@
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
       <c r="O9" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P9" s="9">
         <v>2012</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="R9" s="9"/>
       <c r="S9" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="T9" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="U9" s="9" t="s">
         <v>88</v>
       </c>
       <c r="V9" s="9"/>
       <c r="W9" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="X9" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Y9" s="11">
         <v>2015</v>
       </c>
       <c r="Z9" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AA9" s="11"/>
       <c r="AB9" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AC9" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AD9" s="11" t="s">
         <v>88</v>
@@ -2249,13 +2262,13 @@
         <v>5</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D10" s="9">
         <v>2011</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9" t="s">
@@ -2276,20 +2289,20 @@
       </c>
       <c r="M10" s="11"/>
       <c r="N10" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="P10" s="9">
         <v>2013</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="R10" s="9"/>
       <c r="S10" s="9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="T10" s="9"/>
       <c r="U10" s="9" t="s">
@@ -2308,10 +2321,10 @@
       </c>
       <c r="AA10" s="16"/>
       <c r="AB10" s="16" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="AC10" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AD10" s="16" t="s">
         <v>88</v>
@@ -2319,13 +2332,13 @@
       <c r="AE10" s="11"/>
       <c r="AF10" s="11"/>
       <c r="AG10" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="AH10" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="AI10" s="9" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="AJ10" s="9"/>
       <c r="AK10" s="9" t="s">
@@ -2341,13 +2354,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D11" s="9">
         <v>2011</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9" t="s">
@@ -2368,20 +2381,20 @@
       </c>
       <c r="M11" s="11"/>
       <c r="N11" s="11" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="P11" s="9">
         <v>2011</v>
       </c>
       <c r="Q11" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R11" s="9"/>
       <c r="S11" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="T11" s="9"/>
       <c r="U11" s="9" t="s">
@@ -2400,10 +2413,10 @@
       </c>
       <c r="AA11" s="16"/>
       <c r="AB11" s="16" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="AC11" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AD11" s="16" t="s">
         <v>88</v>
@@ -2411,13 +2424,13 @@
       <c r="AE11" s="11"/>
       <c r="AF11" s="11"/>
       <c r="AG11" s="9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AH11" s="9">
         <v>2011</v>
       </c>
       <c r="AI11" s="9" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="AJ11" s="9"/>
       <c r="AK11" s="9" t="s">
@@ -2433,13 +2446,13 @@
         <v>18</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D12" s="9">
         <v>2011</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9" t="s">
@@ -2460,7 +2473,7 @@
       </c>
       <c r="M12" s="11"/>
       <c r="N12" s="11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
@@ -2482,10 +2495,10 @@
       </c>
       <c r="AA12" s="16"/>
       <c r="AB12" s="16" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="AC12" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AD12" s="16" t="s">
         <v>88</v>
@@ -2493,11 +2506,11 @@
       <c r="AE12" s="11"/>
       <c r="AF12" s="11"/>
       <c r="AG12" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="AH12" s="9"/>
       <c r="AI12" s="9" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="AJ12" s="9"/>
       <c r="AK12" s="9" t="s">
@@ -2507,7 +2520,7 @@
     </row>
     <row r="13" spans="1:38" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B13" s="30"/>
       <c r="C13" s="30"/>
@@ -2585,10 +2598,10 @@
       <c r="AE14" s="11"/>
       <c r="AF14" s="11"/>
       <c r="AG14" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AH14" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="AI14" s="9"/>
       <c r="AJ14" s="9"/>
@@ -2597,10 +2610,10 @@
     </row>
     <row r="15" spans="1:38" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>

</xml_diff>

<commit_message>
note about bh injuries
</commit_message>
<xml_diff>
--- a/project_mgmt/case_cities_data.xlsx
+++ b/project_mgmt/case_cities_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="209">
   <si>
     <t xml:space="preserve">Location</t>
   </si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t xml:space="preserve">Openly available </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data are aggregated over six years. With additional extraction we could get year by year but it’s not worth it right now.</t>
   </si>
   <si>
     <t xml:space="preserve">Colombia</t>
@@ -784,8 +787,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor rgb="FFFFFF99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFB4C7E7"/>
-        <bgColor rgb="FF99CCFF"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -794,34 +803,13 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor rgb="FFFFFF99"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -969,7 +957,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -996,13 +984,7 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -1011,15 +993,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1027,15 +1009,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1043,31 +1025,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="5" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="5" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="5" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="6" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1075,31 +1057,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="7" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="8" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="8" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="8" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="7" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="9" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1107,49 +1089,47 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="11" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="12" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="12" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="12" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="11" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="12" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="11" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="11" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="13" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in 40% - Accent5" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Note" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Input" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -1168,7 +1148,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFB2B2B2"/>
+      <rgbColor rgb="FFB4C7E7"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -1177,7 +1157,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0563C1"/>
-      <rgbColor rgb="FFB4C7E7"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1222,20 +1202,20 @@
   </sheetPr>
   <dimension ref="A1:AL16"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="Z3" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="Y3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="Z1" activeCellId="0" sqref="Z1"/>
+      <selection pane="topRight" activeCell="Y1" activeCellId="0" sqref="Y1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AK11" activeCellId="0" sqref="AK11"/>
+      <selection pane="bottomRight" activeCell="AL5" activeCellId="0" sqref="AL5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="38" min="3" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="39" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="3" style="0" width="18.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="39" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1716,23 +1696,25 @@
       <c r="AK5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AL5" s="15"/>
+      <c r="AL5" s="15" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="62.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D6" s="19" t="n">
         <v>2017</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>24</v>
@@ -1762,37 +1744,37 @@
         <v>2015</v>
       </c>
       <c r="Q6" s="19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="R6" s="19"/>
       <c r="S6" s="19" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="T6" s="19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="U6" s="19" t="s">
         <v>77</v>
       </c>
       <c r="V6" s="19"/>
       <c r="W6" s="19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="X6" s="21" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="Y6" s="21" t="n">
         <v>2015</v>
       </c>
       <c r="Z6" s="21" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AA6" s="21"/>
       <c r="AB6" s="21" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AC6" s="21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AD6" s="21" t="s">
         <v>77</v>
@@ -1800,16 +1782,16 @@
       <c r="AE6" s="21"/>
       <c r="AF6" s="21"/>
       <c r="AG6" s="19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AH6" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AI6" s="19" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AJ6" s="19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AK6" s="19" t="s">
         <v>25</v>
@@ -1818,19 +1800,19 @@
     </row>
     <row r="7" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>24</v>
@@ -1860,24 +1842,24 @@
         <v>2017</v>
       </c>
       <c r="Q7" s="19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="R7" s="19"/>
       <c r="S7" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="T7" s="19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="U7" s="19" t="s">
         <v>77</v>
       </c>
       <c r="V7" s="19"/>
       <c r="W7" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="X7" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="Y7" s="21" t="n">
         <v>2014</v>
@@ -1887,7 +1869,7 @@
       </c>
       <c r="AA7" s="21"/>
       <c r="AB7" s="21" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AC7" s="13" t="s">
         <v>37</v>
@@ -1906,19 +1888,19 @@
     </row>
     <row r="8" customFormat="false" ht="91.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D8" s="19" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F8" s="19" t="s">
         <v>24</v>
@@ -1945,40 +1927,40 @@
         <v>68</v>
       </c>
       <c r="P8" s="19" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Q8" s="19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="R8" s="19"/>
       <c r="S8" s="19" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="T8" s="19" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="U8" s="19" t="s">
         <v>77</v>
       </c>
       <c r="V8" s="19"/>
       <c r="W8" s="19" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="X8" s="21" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="Y8" s="21" t="n">
         <v>2013</v>
       </c>
       <c r="Z8" s="21" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AA8" s="21"/>
       <c r="AB8" s="21" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AC8" s="21" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AD8" s="21" t="s">
         <v>77</v>
@@ -1994,19 +1976,19 @@
     </row>
     <row r="9" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D9" s="19" t="n">
         <v>2017</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F9" s="19" t="s">
         <v>24</v>
@@ -2036,37 +2018,37 @@
         <v>2012</v>
       </c>
       <c r="Q9" s="19" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="R9" s="19"/>
       <c r="S9" s="19" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="T9" s="19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U9" s="19" t="s">
         <v>77</v>
       </c>
       <c r="V9" s="19"/>
       <c r="W9" s="19" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="X9" s="21" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="Y9" s="21" t="n">
         <v>2015</v>
       </c>
       <c r="Z9" s="21" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AA9" s="21"/>
       <c r="AB9" s="21" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AC9" s="21" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AD9" s="21" t="s">
         <v>77</v>
@@ -2082,19 +2064,19 @@
     </row>
     <row r="10" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D10" s="19" t="n">
         <v>2011</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F10" s="19"/>
       <c r="G10" s="19" t="s">
@@ -2115,20 +2097,20 @@
       </c>
       <c r="M10" s="21"/>
       <c r="N10" s="21" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="O10" s="19" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="P10" s="19" t="n">
         <v>2013</v>
       </c>
       <c r="Q10" s="19" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="R10" s="19"/>
       <c r="S10" s="19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="T10" s="19"/>
       <c r="U10" s="19" t="s">
@@ -2147,7 +2129,7 @@
       </c>
       <c r="AA10" s="13"/>
       <c r="AB10" s="13" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AC10" s="13" t="s">
         <v>37</v>
@@ -2158,13 +2140,13 @@
       <c r="AE10" s="21"/>
       <c r="AF10" s="21"/>
       <c r="AG10" s="19" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="AH10" s="19" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AI10" s="19" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AJ10" s="19"/>
       <c r="AK10" s="19" t="s">
@@ -2174,19 +2156,19 @@
     </row>
     <row r="11" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D11" s="19" t="n">
         <v>2011</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F11" s="19"/>
       <c r="G11" s="19" t="s">
@@ -2207,20 +2189,20 @@
       </c>
       <c r="M11" s="21"/>
       <c r="N11" s="21" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="O11" s="19" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="P11" s="19" t="n">
         <v>2011</v>
       </c>
       <c r="Q11" s="19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="R11" s="19"/>
       <c r="S11" s="19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="T11" s="19"/>
       <c r="U11" s="19" t="s">
@@ -2239,7 +2221,7 @@
       </c>
       <c r="AA11" s="13"/>
       <c r="AB11" s="13" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AC11" s="13" t="s">
         <v>37</v>
@@ -2250,13 +2232,13 @@
       <c r="AE11" s="21"/>
       <c r="AF11" s="21"/>
       <c r="AG11" s="19" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AH11" s="19" t="n">
         <v>2011</v>
       </c>
       <c r="AI11" s="19" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AJ11" s="19"/>
       <c r="AK11" s="19" t="s">
@@ -2266,19 +2248,19 @@
     </row>
     <row r="12" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D12" s="19" t="n">
         <v>2011</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F12" s="19"/>
       <c r="G12" s="19" t="s">
@@ -2299,7 +2281,7 @@
       </c>
       <c r="M12" s="21"/>
       <c r="N12" s="21" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="O12" s="19"/>
       <c r="P12" s="19"/>
@@ -2321,7 +2303,7 @@
       </c>
       <c r="AA12" s="13"/>
       <c r="AB12" s="13" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AC12" s="13" t="s">
         <v>37</v>
@@ -2332,11 +2314,11 @@
       <c r="AE12" s="21"/>
       <c r="AF12" s="21"/>
       <c r="AG12" s="19" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="AH12" s="19"/>
       <c r="AI12" s="19" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AJ12" s="19"/>
       <c r="AK12" s="19" t="s">
@@ -2346,7 +2328,7 @@
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="25" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
@@ -2388,10 +2370,10 @@
     </row>
     <row r="14" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
@@ -2424,10 +2406,10 @@
       <c r="AE14" s="21"/>
       <c r="AF14" s="21"/>
       <c r="AG14" s="19" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="AH14" s="19" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AI14" s="19"/>
       <c r="AJ14" s="19"/>
@@ -2436,10 +2418,10 @@
     </row>
     <row r="15" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="17" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
@@ -2480,10 +2462,10 @@
     </row>
     <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="26" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
@@ -2547,7 +2529,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2562,227 +2544,227 @@
   </sheetPr>
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.6734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D23" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Leandro updated PA datasets
</commit_message>
<xml_diff>
--- a/project_mgmt/case_cities_data.xlsx
+++ b/project_mgmt/case_cities_data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RStudio Projects\ITHIM-R\project_mgmt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12772EEF-06B8-4AB2-AE97-77EF7BCA1057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16095" windowHeight="5415" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="242">
   <si>
     <t>Location</t>
   </si>
@@ -796,11 +797,29 @@
   <si>
     <t>BA: 44 commerical : 27 (293 sample )</t>
   </si>
+  <si>
+    <t>Only LTPA is provided. Sao Paulo occ PA data can be used.</t>
+  </si>
+  <si>
+    <t>V:\Studies\MOVED\HealthImpact\Data\TIGTHAT\Brazil\Belo Horizonte\Physical activity\Process PA data.R</t>
+  </si>
+  <si>
+    <t>V:\Studies\MOVED\HealthImpact\Data\TIGTHAT\Colombia\Bogota\Physical activity\Process PA data.R</t>
+  </si>
+  <si>
+    <t>V:\Studies\MOVED\HealthImpact\Data\TIGTHAT\Argentina\WP3-PA\Process PA data.R</t>
+  </si>
+  <si>
+    <t>Only total MVPA can be calculated. However, survey participants indicated in which PA domains they engaged last week (same time of PA data).</t>
+  </si>
+  <si>
+    <t>V:\Studies\MOVED\HealthImpact\Data\TIGTHAT\Chile\Physical activity\Process PA data.R</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1578,14 +1597,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="R5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AS8" sqref="AS8"/>
+      <selection pane="bottomRight" activeCell="AF9" sqref="AF9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2099,9 +2118,11 @@
         <v>77</v>
       </c>
       <c r="AE5" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF5" s="18"/>
+        <v>26</v>
+      </c>
+      <c r="AF5" s="18" t="s">
+        <v>237</v>
+      </c>
       <c r="AG5" s="18"/>
       <c r="AH5" s="16" t="s">
         <v>79</v>
@@ -2202,10 +2223,14 @@
         <v>95</v>
       </c>
       <c r="AE6" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF6" s="18"/>
-      <c r="AG6" s="18"/>
+        <v>26</v>
+      </c>
+      <c r="AF6" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="AG6" s="18" t="s">
+        <v>236</v>
+      </c>
       <c r="AH6" s="16" t="s">
         <v>96</v>
       </c>
@@ -2309,7 +2334,7 @@
         <v>38</v>
       </c>
       <c r="AE7" s="18" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="AF7" s="18"/>
       <c r="AG7" s="18"/>
@@ -2422,10 +2447,14 @@
         <v>130</v>
       </c>
       <c r="AE8" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF8" s="18"/>
-      <c r="AG8" s="18"/>
+        <v>26</v>
+      </c>
+      <c r="AF8" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="AG8" s="18" t="s">
+        <v>240</v>
+      </c>
       <c r="AH8" s="24" t="s">
         <v>131</v>
       </c>
@@ -2526,10 +2555,14 @@
         <v>145</v>
       </c>
       <c r="AE9" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF9" s="18"/>
-      <c r="AG9" s="18"/>
+        <v>26</v>
+      </c>
+      <c r="AF9" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="AG9" s="18" t="s">
+        <v>240</v>
+      </c>
       <c r="AH9" s="16" t="s">
         <v>146</v>
       </c>
@@ -2633,7 +2666,7 @@
         <v>38</v>
       </c>
       <c r="AE10" s="10" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="AF10" s="18"/>
       <c r="AG10" s="18"/>
@@ -2728,7 +2761,7 @@
         <v>38</v>
       </c>
       <c r="AE11" s="10" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="AF11" s="18"/>
       <c r="AG11" s="18"/>
@@ -2829,7 +2862,7 @@
         <v>38</v>
       </c>
       <c r="AE12" s="10" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="AF12" s="18"/>
       <c r="AG12" s="18"/>
@@ -3040,17 +3073,17 @@
     <mergeCell ref="Y1:AG1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1"/>
-    <hyperlink ref="K4" r:id="rId2"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="K5" r:id="rId4"/>
-    <hyperlink ref="K6" r:id="rId5"/>
-    <hyperlink ref="K7" r:id="rId6"/>
-    <hyperlink ref="K8" r:id="rId7"/>
-    <hyperlink ref="K9" r:id="rId8"/>
-    <hyperlink ref="K10" r:id="rId9"/>
-    <hyperlink ref="K11" r:id="rId10"/>
-    <hyperlink ref="K12" r:id="rId11"/>
+    <hyperlink ref="K3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="K5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="K6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="K7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="K8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="K9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="K10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="K11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="K12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
@@ -3058,7 +3091,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>